<commit_message>
Emparejamiento por "Debe" y "Haber" no cero: Si una fila tiene 0 en una de las columnas ("Debe" o "Haber"), pero tiene un valor válido en la otra, se empareja con la fila correspondiente que tenga un valor coincidente. Por ejemplo, si una fila tiene Debe = 0 y Haber = 100, se emparejará con una fila donde Debe = 100 y Haber = 0.
Revisión de filas con 0: Se siguen considerando las filas con 0 en "Debe" o "Haber", pero ahora solo se ignorarán las celdas con valor 0, no la fila completa.
</commit_message>
<xml_diff>
--- a/informes/no_punteados.xlsx
+++ b/informes/no_punteados.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,6 +524,274 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
+        <v>45611</v>
+      </c>
+      <c r="B2" t="n">
+        <v>4042080</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Creación Anticipo 409112186/1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4824</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>IMEDISA ARTES GRAFICAS, S.L.U.</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>361.94</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-2470.21</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>sandra</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L2" t="n">
+        <v>438004824</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>409112186/1</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>45616</v>
+      </c>
+      <c r="B3" t="n">
+        <v>4042912</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Compensación Anticipo 409112186/1</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>4824</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>IMEDISA ARTES GRAFICAS, S.L.U.</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>105.9</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-721.59</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>MIREA93</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L3" t="n">
+        <v>438004824</v>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>409112186/1</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>45621</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4043419</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Compensación Anticipo 409112186/1</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>4824</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>IMEDISA ARTES GRAFICAS, S.L.U.</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>256.04</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-465.55</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>M.Jose</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L4" t="n">
+        <v>438004824</v>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>409112186/1</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>45656</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4047697</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Creación Anticipo 409127725/1</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>4824</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>IMEDISA ARTES GRAFICAS, S.L.U.</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>738.84</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-738.84</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>sandra</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>438004824</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>yes</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>409127725/1</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>